<commit_message>
Cambio toda la interfaz visual y agrego logo
</commit_message>
<xml_diff>
--- a/data/Villa Atuel S.A/revision_villa_atuel_s.a_20250723.xlsx
+++ b/data/Villa Atuel S.A/revision_villa_atuel_s.a_20250723.xlsx
@@ -468,12 +468,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Picado</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Sin modificaciones</t>
+          <t>ar{kgnaer{hk</t>
         </is>
       </c>
     </row>
@@ -490,12 +490,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Comido</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>aojsfbnañjelr</t>
+          <t>Sin modificaciones</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Agrego README y TODO y agrego assets como ICO
</commit_message>
<xml_diff>
--- a/data/Villa Atuel S.A/revision_villa_atuel_s.a_20250723.xlsx
+++ b/data/Villa Atuel S.A/revision_villa_atuel_s.a_20250723.xlsx
@@ -468,12 +468,12 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Picado</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>ar{kgnaer{hk</t>
+          <t>Sin modificaciones</t>
         </is>
       </c>
     </row>
@@ -490,12 +490,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Normal</t>
+          <t>Comido</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Sin modificaciones</t>
+          <t>asfvarfg</t>
         </is>
       </c>
     </row>

</xml_diff>